<commit_message>
now it can be started on less then maximum threads + edit excel a bit
</commit_message>
<xml_diff>
--- a/Lab1_excel.xlsx
+++ b/Lab1_excel.xlsx
@@ -1,32 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darya\CLionProjects\LabMPITasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A441107-CCA5-4B30-B1E7-026071041E34}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C62289-C514-48BA-B51D-CFE67760FE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{FC483C37-E4EE-4DFF-B7FA-F23CF211A9C2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FC483C37-E4EE-4DFF-B7FA-F23CF211A9C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>thread number</t>
   </si>
@@ -229,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -245,6 +253,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -263,9 +274,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -300,7 +317,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.3707086929543845E-2"/>
+          <c:y val="2.0331370294426689E-2"/>
+          <c:w val="0.91629291307045613"/>
+          <c:h val="0.78873445927532237"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -367,10 +394,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.9822902878151871</c:v>
+                  <c:v>0.67494731345232095</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.6210114335026695</c:v>
+                  <c:v>1.6104252295689769</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3.9338364024382453</c:v>
@@ -668,6 +695,648 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>parallel speed-up</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$G$40:$G$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$40:$K$42</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.5582733555019761</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24570944162761274</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4206158187401456</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6D5D-4986-8F28-B599C9EF9E83}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="486612975"/>
+        <c:axId val="486617967"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="486612975"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="486617967"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="486617967"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="486612975"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$62</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>parallel speed-up</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$F$63:$F$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$63:$J$65</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.47811860030273212</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.73092855967816817</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.6300091727340558</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-58B0-4323-9864-5D8534F0EE11}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="254679183"/>
+        <c:axId val="429482175"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="254679183"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="429482175"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="429482175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="254679183"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -708,7 +1377,1119 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1270,8 +3051,8 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>198801</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>808401</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>38563</xdr:rowOff>
     </xdr:to>
@@ -1949,8 +3730,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="11056620" cy="921214"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -2343,7 +4124,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -2488,6 +4269,78 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1287780</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77573B2F-7286-423B-B2ED-B85FD1D48F05}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1280160</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A14F2894-5C96-4D54-9BCE-05BDCBC9C140}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2788,10 +4641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0553C8DC-BA51-47AF-989B-7D727882C3D6}">
-  <dimension ref="A1:L59"/>
+  <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2802,23 +4655,27 @@
     <col min="5" max="5" width="26.88671875" customWidth="1"/>
     <col min="6" max="6" width="34.88671875" customWidth="1"/>
     <col min="7" max="7" width="26.44140625" customWidth="1"/>
+    <col min="8" max="8" width="20.77734375" customWidth="1"/>
+    <col min="9" max="9" width="25.44140625" customWidth="1"/>
+    <col min="10" max="10" width="24.109375" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="62.4" customHeight="1">
-      <c r="A1" s="15"/>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="9"/>
+      <c r="B1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
     </row>
     <row r="2" spans="1:12" ht="21" customHeight="1">
       <c r="B2" s="2" t="s">
@@ -2840,8 +4697,8 @@
       <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="7">
-        <v>3.08983E-2</v>
+      <c r="C3" s="4">
+        <v>0.18230460000000001</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="4">
@@ -2849,7 +4706,7 @@
       </c>
       <c r="F3" s="6">
         <f>E3/C3</f>
-        <v>3.9822902878151871</v>
+        <v>0.67494731345232095</v>
       </c>
       <c r="G3" s="6"/>
     </row>
@@ -2858,7 +4715,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="7">
-        <v>2.7926699999999999E-2</v>
+        <v>6.2792669999999995E-2</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="4">
@@ -2866,7 +4723,7 @@
       </c>
       <c r="F4" s="6">
         <f t="shared" ref="F4:F9" si="0">E4/C4</f>
-        <v>3.6210114335026695</v>
+        <v>1.6104252295689769</v>
       </c>
       <c r="G4" s="6"/>
     </row>
@@ -2959,39 +4816,109 @@
       <c r="B10" s="1">
         <v>9</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="11"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:12">
       <c r="B11" s="3">
         <v>10</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
     </row>
     <row r="34" spans="1:12" ht="31.2">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="16" t="s">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="G39" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="G40" s="1">
+        <v>2</v>
+      </c>
+      <c r="H40" s="18">
+        <v>2.6600122451782199E-2</v>
+      </c>
+      <c r="I40" s="18"/>
+      <c r="J40" s="19">
+        <v>1.4850139617919899E-2</v>
+      </c>
+      <c r="K40" s="6">
+        <f>J40/H40</f>
+        <v>0.5582733555019761</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="G41" s="1">
+        <v>3</v>
+      </c>
+      <c r="H41" s="18">
+        <v>4.4718503952026402E-2</v>
+      </c>
+      <c r="I41" s="18"/>
+      <c r="J41" s="19">
+        <v>1.0987758636474601E-2</v>
+      </c>
+      <c r="K41" s="6">
+        <f>J41/H41</f>
+        <v>0.24570944162761274</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="G42" s="1">
+        <v>4</v>
+      </c>
+      <c r="H42" s="18">
+        <v>1.43635272979736E-2</v>
+      </c>
+      <c r="I42" s="18"/>
+      <c r="J42" s="19">
+        <v>2.0405054092407199E-2</v>
+      </c>
+      <c r="K42" s="6">
+        <f>J42/H42</f>
+        <v>1.4206158187401456</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="G43" s="3"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="6"/>
     </row>
     <row r="44" spans="1:12">
       <c r="F44" s="8" t="s">
@@ -3000,20 +4927,83 @@
     </row>
     <row r="52" spans="1:12" ht="66" customHeight="1"/>
     <row r="59" spans="1:12" ht="36.6">
-      <c r="A59" s="15"/>
-      <c r="B59" s="17" t="s">
+      <c r="A59" s="9"/>
+      <c r="B59" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15"/>
-      <c r="G59" s="15"/>
-      <c r="H59" s="15"/>
-      <c r="I59" s="15"/>
-      <c r="J59" s="15"/>
-      <c r="K59" s="15"/>
-      <c r="L59" s="15"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="9"/>
+      <c r="K59" s="9"/>
+      <c r="L59" s="9"/>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="F62" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="F63" s="1">
+        <v>2</v>
+      </c>
+      <c r="G63" s="18">
+        <v>2.1421432495117201E-2</v>
+      </c>
+      <c r="H63" s="18"/>
+      <c r="I63" s="19">
+        <v>1.0241985321044899E-2</v>
+      </c>
+      <c r="J63" s="6">
+        <f>I63/G63</f>
+        <v>0.47811860030273212</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="F64" s="1">
+        <v>3</v>
+      </c>
+      <c r="G64" s="18">
+        <v>1.5942335128784201E-2</v>
+      </c>
+      <c r="H64" s="18"/>
+      <c r="I64" s="19">
+        <v>1.16527080535889E-2</v>
+      </c>
+      <c r="J64" s="6">
+        <f>I64/G64</f>
+        <v>0.73092855967816817</v>
+      </c>
+    </row>
+    <row r="65" spans="6:10">
+      <c r="F65" s="1">
+        <v>4</v>
+      </c>
+      <c r="G65" s="18">
+        <v>1.6634941101074201E-2</v>
+      </c>
+      <c r="H65" s="18"/>
+      <c r="I65" s="19">
+        <v>7.7019929885864299E-2</v>
+      </c>
+      <c r="J65" s="6">
+        <f>I65/G65</f>
+        <v>4.6300091727340558</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>